<commit_message>
added all delegation variable definitions
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/SurveyResults/Survey Delegation Variables.xlsx
+++ b/dashboard-ui/src/components/SurveyResults/Survey Delegation Variables.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79D1ED4B-8FC1-4022-B818-AAEC61DC9975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{675A8911-BEA1-4323-9B15-3BC35ADE7F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
   <si>
     <t>Variables</t>
   </si>
@@ -147,6 +147,12 @@
     <t>The total time it took the participant to go through the last page of the survey</t>
   </si>
   <si>
+    <t>The participant's response to "How much experience did you have with VR Gaming before today?"</t>
+  </si>
+  <si>
+    <t>The total time it took the participant to read through the instructions</t>
+  </si>
+  <si>
     <t>X refers to the block number, Y refers to the DM number the participant saw. For Eval 4 and 5, participants saw 4 blocks with 2-3 DMs each. The following columns describe each page of the survey using this BX_DMY format.</t>
   </si>
   <si>
@@ -213,7 +219,10 @@
     <t>Levels</t>
   </si>
   <si>
-    <t>1.1, 1.2, 1.3, 2, 3, 4, 5</t>
+    <t>4, 5</t>
+  </si>
+  <si>
+    <t>0 - None at all \n 1 - I have used it, but not often \n 2 - I use it occasionally \n 3 - I use it often \n 4 - I use it all the time</t>
   </si>
   <si>
     <t>B1_DM1, B1_DM2, B1_DM3, B2_DM1, B2_DM2, etc.</t>
@@ -613,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -745,119 +754,129 @@
       <c r="G2" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="J2" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AD2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE2" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="126" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E3" s="2"/>
+      <c r="H3" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="J3" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
+  <printOptions horizontalCentered="1" verticalCentered="1" headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>